<commit_message>
CF1/CA1: Replaced Noncontiguous flag with Leap pre/late fill check
</commit_message>
<xml_diff>
--- a/MGen/cf1-cor.xlsx
+++ b/MGen/cf1-cor.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cf1-cor" sheetId="1" r:id="rId1"/>
     <sheet name="Лист1" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="85">
   <si>
     <t>Strict</t>
   </si>
@@ -246,6 +247,30 @@
   </si>
   <si>
     <t>Prepared unfilled 3rd</t>
+  </si>
+  <si>
+    <t>No flag</t>
+  </si>
+  <si>
+    <t>Pre/late</t>
+  </si>
+  <si>
+    <t>Unfilled</t>
+  </si>
+  <si>
+    <t>Local unfilled</t>
+  </si>
+  <si>
+    <t>Global unfilled</t>
+  </si>
+  <si>
+    <t>3rd prepared</t>
+  </si>
+  <si>
+    <t>No matter</t>
+  </si>
+  <si>
+    <t>3rd prepared unfilled</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1139,7 @@
   <dimension ref="A1:AM37"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:AM37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1413,19 +1438,19 @@
         <v>885002</v>
       </c>
       <c r="R3">
-        <v>1385576</v>
+        <v>919657</v>
       </c>
       <c r="S3">
-        <v>602706</v>
+        <v>385994</v>
       </c>
       <c r="T3">
         <v>226080</v>
       </c>
       <c r="U3">
-        <v>1022843</v>
+        <v>598880</v>
       </c>
       <c r="V3">
-        <v>489666</v>
+        <v>284466</v>
       </c>
       <c r="W3">
         <v>212789</v>
@@ -1532,19 +1557,19 @@
         <v>4596</v>
       </c>
       <c r="R4">
-        <v>13543</v>
+        <v>9415</v>
       </c>
       <c r="S4">
-        <v>4783</v>
+        <v>2962</v>
       </c>
       <c r="T4">
         <v>1845</v>
       </c>
       <c r="U4">
-        <v>9466</v>
+        <v>6707</v>
       </c>
       <c r="V4">
-        <v>2875</v>
+        <v>1224</v>
       </c>
       <c r="W4">
         <v>1655</v>
@@ -1651,19 +1676,19 @@
         <v>111892</v>
       </c>
       <c r="R5">
-        <v>104426</v>
+        <v>78965</v>
       </c>
       <c r="S5">
-        <v>28619</v>
+        <v>20155</v>
       </c>
       <c r="T5">
         <v>8594</v>
       </c>
       <c r="U5">
-        <v>66134</v>
+        <v>43973</v>
       </c>
       <c r="V5">
-        <v>23592</v>
+        <v>16640</v>
       </c>
       <c r="W5">
         <v>7002</v>
@@ -1770,7 +1795,7 @@
         <v>54</v>
       </c>
       <c r="R6">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="S6">
         <v>6</v>
@@ -1779,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="U6">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="V6">
         <v>6</v>
@@ -1889,19 +1914,19 @@
         <v>828657</v>
       </c>
       <c r="R7">
-        <v>1571704</v>
+        <v>903782</v>
       </c>
       <c r="S7">
-        <v>935062</v>
+        <v>485222</v>
       </c>
       <c r="T7">
         <v>478516</v>
       </c>
       <c r="U7">
-        <v>1284153</v>
+        <v>624301</v>
       </c>
       <c r="V7">
-        <v>784349</v>
+        <v>379976</v>
       </c>
       <c r="W7">
         <v>423641</v>
@@ -2008,19 +2033,19 @@
         <v>193383</v>
       </c>
       <c r="R8">
-        <v>349379</v>
+        <v>203421</v>
       </c>
       <c r="S8">
-        <v>201005</v>
+        <v>118943</v>
       </c>
       <c r="T8">
         <v>87591</v>
       </c>
       <c r="U8">
-        <v>297227</v>
+        <v>158709</v>
       </c>
       <c r="V8">
-        <v>166527</v>
+        <v>83196</v>
       </c>
       <c r="W8">
         <v>85817</v>
@@ -2127,19 +2152,19 @@
         <v>345511</v>
       </c>
       <c r="R9">
-        <v>534828</v>
+        <v>366623</v>
       </c>
       <c r="S9">
-        <v>219076</v>
+        <v>145371</v>
       </c>
       <c r="T9">
         <v>75771</v>
       </c>
       <c r="U9">
-        <v>379907</v>
+        <v>231266</v>
       </c>
       <c r="V9">
-        <v>169441</v>
+        <v>103503</v>
       </c>
       <c r="W9">
         <v>67806</v>
@@ -2246,19 +2271,19 @@
         <v>596578</v>
       </c>
       <c r="R10">
-        <v>1014015</v>
+        <v>614725</v>
       </c>
       <c r="S10">
-        <v>570854</v>
+        <v>317818</v>
       </c>
       <c r="T10">
         <v>268552</v>
       </c>
       <c r="U10">
-        <v>821880</v>
+        <v>431756</v>
       </c>
       <c r="V10">
-        <v>471285</v>
+        <v>260332</v>
       </c>
       <c r="W10">
         <v>221029</v>
@@ -2365,19 +2390,19 @@
         <v>200403</v>
       </c>
       <c r="R11">
-        <v>285946</v>
+        <v>110550</v>
       </c>
       <c r="S11">
-        <v>223660</v>
+        <v>113134</v>
       </c>
       <c r="T11">
         <v>120674</v>
       </c>
       <c r="U11">
-        <v>299190</v>
+        <v>143951</v>
       </c>
       <c r="V11">
-        <v>195265</v>
+        <v>99008</v>
       </c>
       <c r="W11">
         <v>103545</v>
@@ -2484,19 +2509,19 @@
         <v>502549</v>
       </c>
       <c r="R12">
-        <v>709616</v>
+        <v>400082</v>
       </c>
       <c r="S12">
-        <v>398268</v>
+        <v>200484</v>
       </c>
       <c r="T12">
         <v>209208</v>
       </c>
       <c r="U12">
-        <v>643018</v>
+        <v>294731</v>
       </c>
       <c r="V12">
-        <v>401647</v>
+        <v>189416</v>
       </c>
       <c r="W12">
         <v>222827</v>
@@ -2603,19 +2628,19 @@
         <v>1735047</v>
       </c>
       <c r="R13">
-        <v>2927792</v>
+        <v>1856104</v>
       </c>
       <c r="S13">
-        <v>1458486</v>
+        <v>867306</v>
       </c>
       <c r="T13">
         <v>625084</v>
       </c>
       <c r="U13">
-        <v>2247192</v>
+        <v>1249595</v>
       </c>
       <c r="V13">
-        <v>1176991</v>
+        <v>649708</v>
       </c>
       <c r="W13">
         <v>549379</v>
@@ -2722,19 +2747,19 @@
         <v>833666</v>
       </c>
       <c r="R14">
-        <v>1375144</v>
+        <v>850698</v>
       </c>
       <c r="S14">
-        <v>710540</v>
+        <v>406622</v>
       </c>
       <c r="T14">
         <v>323796</v>
       </c>
       <c r="U14">
-        <v>1106387</v>
+        <v>590127</v>
       </c>
       <c r="V14">
-        <v>611482</v>
+        <v>321982</v>
       </c>
       <c r="W14">
         <v>304080</v>
@@ -2841,19 +2866,19 @@
         <v>963779</v>
       </c>
       <c r="R15">
-        <v>1699801</v>
+        <v>1133776</v>
       </c>
       <c r="S15">
-        <v>837859</v>
+        <v>513137</v>
       </c>
       <c r="T15">
         <v>347064</v>
       </c>
       <c r="U15">
-        <v>1233681</v>
+        <v>710035</v>
       </c>
       <c r="V15">
-        <v>616880</v>
+        <v>345958</v>
       </c>
       <c r="W15">
         <v>280316</v>
@@ -2960,19 +2985,19 @@
         <v>1838655</v>
       </c>
       <c r="R16">
-        <v>1436459</v>
+        <v>920886</v>
       </c>
       <c r="S16">
-        <v>718045</v>
+        <v>425882</v>
       </c>
       <c r="T16">
         <v>309436</v>
       </c>
       <c r="U16">
-        <v>1156439</v>
+        <v>623919</v>
       </c>
       <c r="V16">
-        <v>628609</v>
+        <v>376950</v>
       </c>
       <c r="W16">
         <v>263418</v>
@@ -3031,115 +3056,115 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>3131464</v>
+        <v>2007816</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1385576</v>
+        <v>919657</v>
       </c>
       <c r="E17">
-        <v>13543</v>
+        <v>9415</v>
       </c>
       <c r="F17">
-        <v>104426</v>
+        <v>78965</v>
       </c>
       <c r="G17">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H17">
-        <v>1571704</v>
+        <v>903782</v>
       </c>
       <c r="I17">
-        <v>349379</v>
+        <v>203421</v>
       </c>
       <c r="J17">
-        <v>534828</v>
+        <v>366623</v>
       </c>
       <c r="K17">
-        <v>1014015</v>
+        <v>614725</v>
       </c>
       <c r="L17">
-        <v>285946</v>
+        <v>110550</v>
       </c>
       <c r="M17">
-        <v>709616</v>
+        <v>400082</v>
       </c>
       <c r="N17">
-        <v>2927792</v>
+        <v>1856104</v>
       </c>
       <c r="O17">
-        <v>1375144</v>
+        <v>850698</v>
       </c>
       <c r="P17">
-        <v>1699801</v>
+        <v>1133776</v>
       </c>
       <c r="Q17">
-        <v>1436459</v>
+        <v>920886</v>
       </c>
       <c r="R17">
-        <v>3131464</v>
+        <v>2007816</v>
       </c>
       <c r="S17">
-        <v>1537082</v>
+        <v>261344</v>
       </c>
       <c r="T17">
-        <v>645648</v>
+        <v>154498</v>
       </c>
       <c r="U17">
-        <v>1910994</v>
+        <v>635699</v>
       </c>
       <c r="V17">
-        <v>1017265</v>
+        <v>340529</v>
       </c>
       <c r="W17">
-        <v>473324</v>
+        <v>227822</v>
       </c>
       <c r="X17">
-        <v>1561620</v>
+        <v>1007313</v>
       </c>
       <c r="Y17">
-        <v>990650</v>
+        <v>598219</v>
       </c>
       <c r="Z17">
-        <v>2410002</v>
+        <v>1566512</v>
       </c>
       <c r="AA17">
-        <v>3117552</v>
+        <v>1997856</v>
       </c>
       <c r="AB17">
-        <v>3020514</v>
+        <v>1923953</v>
       </c>
       <c r="AC17">
-        <v>320235</v>
+        <v>208496</v>
       </c>
       <c r="AD17">
-        <v>1682463</v>
+        <v>1036125</v>
       </c>
       <c r="AE17">
-        <v>74040</v>
+        <v>46798</v>
       </c>
       <c r="AF17">
-        <v>281320</v>
+        <v>194214</v>
       </c>
       <c r="AG17">
-        <v>324637</v>
+        <v>215385</v>
       </c>
       <c r="AH17">
-        <v>558086</v>
+        <v>391650</v>
       </c>
       <c r="AI17">
-        <v>161184</v>
+        <v>113904</v>
       </c>
       <c r="AJ17">
-        <v>3093580</v>
+        <v>1979168</v>
       </c>
       <c r="AK17">
-        <v>412684</v>
+        <v>245594</v>
       </c>
       <c r="AL17">
-        <v>1947504</v>
+        <v>1227495</v>
       </c>
       <c r="AM17" t="s">
         <v>1</v>
@@ -3150,115 +3175,115 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1537082</v>
+        <v>925730</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>602706</v>
+        <v>385994</v>
       </c>
       <c r="E18">
-        <v>4783</v>
+        <v>2962</v>
       </c>
       <c r="F18">
-        <v>28619</v>
+        <v>20155</v>
       </c>
       <c r="G18">
         <v>6</v>
       </c>
       <c r="H18">
-        <v>935062</v>
+        <v>485222</v>
       </c>
       <c r="I18">
-        <v>201005</v>
+        <v>118943</v>
       </c>
       <c r="J18">
-        <v>219076</v>
+        <v>145371</v>
       </c>
       <c r="K18">
-        <v>570854</v>
+        <v>317818</v>
       </c>
       <c r="L18">
-        <v>223660</v>
+        <v>113134</v>
       </c>
       <c r="M18">
-        <v>398268</v>
+        <v>200484</v>
       </c>
       <c r="N18">
-        <v>1458486</v>
+        <v>867306</v>
       </c>
       <c r="O18">
-        <v>710540</v>
+        <v>406622</v>
       </c>
       <c r="P18">
-        <v>837859</v>
+        <v>513137</v>
       </c>
       <c r="Q18">
-        <v>718045</v>
+        <v>425882</v>
       </c>
       <c r="R18">
-        <v>1537082</v>
+        <v>261344</v>
       </c>
       <c r="S18">
-        <v>1537082</v>
+        <v>925730</v>
       </c>
       <c r="T18">
-        <v>645648</v>
+        <v>34296</v>
       </c>
       <c r="U18">
-        <v>1054606</v>
+        <v>374274</v>
       </c>
       <c r="V18">
-        <v>607266</v>
+        <v>177728</v>
       </c>
       <c r="W18">
-        <v>303334</v>
+        <v>135906</v>
       </c>
       <c r="X18">
-        <v>757029</v>
+        <v>461769</v>
       </c>
       <c r="Y18">
-        <v>558395</v>
+        <v>309440</v>
       </c>
       <c r="Z18">
-        <v>1178570</v>
+        <v>714872</v>
       </c>
       <c r="AA18">
-        <v>1532092</v>
+        <v>921991</v>
       </c>
       <c r="AB18">
-        <v>1506721</v>
+        <v>904541</v>
       </c>
       <c r="AC18">
-        <v>141217</v>
+        <v>89139</v>
       </c>
       <c r="AD18">
-        <v>894078</v>
+        <v>516358</v>
       </c>
       <c r="AE18">
-        <v>43868</v>
+        <v>24570</v>
       </c>
       <c r="AF18">
-        <v>114615</v>
+        <v>76772</v>
       </c>
       <c r="AG18">
-        <v>144673</v>
+        <v>93109</v>
       </c>
       <c r="AH18">
-        <v>204239</v>
+        <v>146380</v>
       </c>
       <c r="AI18">
-        <v>53904</v>
+        <v>39096</v>
       </c>
       <c r="AJ18">
-        <v>1527193</v>
+        <v>918168</v>
       </c>
       <c r="AK18">
-        <v>202422</v>
+        <v>121208</v>
       </c>
       <c r="AL18">
-        <v>1010038</v>
+        <v>592239</v>
       </c>
       <c r="AM18" t="s">
         <v>1</v>
@@ -3317,19 +3342,19 @@
         <v>309436</v>
       </c>
       <c r="R19">
-        <v>645648</v>
+        <v>154498</v>
       </c>
       <c r="S19">
-        <v>645648</v>
+        <v>34296</v>
       </c>
       <c r="T19">
         <v>645648</v>
       </c>
       <c r="U19">
-        <v>464154</v>
+        <v>199536</v>
       </c>
       <c r="V19">
-        <v>314998</v>
+        <v>152460</v>
       </c>
       <c r="W19">
         <v>177210</v>
@@ -3388,115 +3413,115 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>2364652</v>
+        <v>1336971</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1022843</v>
+        <v>598880</v>
       </c>
       <c r="E20">
-        <v>9466</v>
+        <v>6707</v>
       </c>
       <c r="F20">
-        <v>66134</v>
+        <v>43973</v>
       </c>
       <c r="G20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H20">
-        <v>1284153</v>
+        <v>624301</v>
       </c>
       <c r="I20">
-        <v>297227</v>
+        <v>158709</v>
       </c>
       <c r="J20">
-        <v>379907</v>
+        <v>231266</v>
       </c>
       <c r="K20">
-        <v>821880</v>
+        <v>431756</v>
       </c>
       <c r="L20">
-        <v>299190</v>
+        <v>143951</v>
       </c>
       <c r="M20">
-        <v>643018</v>
+        <v>294731</v>
       </c>
       <c r="N20">
-        <v>2247192</v>
+        <v>1249595</v>
       </c>
       <c r="O20">
-        <v>1106387</v>
+        <v>590127</v>
       </c>
       <c r="P20">
-        <v>1233681</v>
+        <v>710035</v>
       </c>
       <c r="Q20">
-        <v>1156439</v>
+        <v>623919</v>
       </c>
       <c r="R20">
-        <v>1910994</v>
+        <v>635699</v>
       </c>
       <c r="S20">
-        <v>1054606</v>
+        <v>374274</v>
       </c>
       <c r="T20">
-        <v>464154</v>
+        <v>199536</v>
       </c>
       <c r="U20">
-        <v>2364652</v>
+        <v>1336971</v>
       </c>
       <c r="V20">
-        <v>1211335</v>
+        <v>119776</v>
       </c>
       <c r="W20">
-        <v>555003</v>
+        <v>63926</v>
       </c>
       <c r="X20">
-        <v>1215681</v>
+        <v>683599</v>
       </c>
       <c r="Y20">
-        <v>822933</v>
+        <v>427417</v>
       </c>
       <c r="Z20">
-        <v>1832247</v>
+        <v>1037925</v>
       </c>
       <c r="AA20">
-        <v>2357448</v>
+        <v>1331593</v>
       </c>
       <c r="AB20">
-        <v>2293942</v>
+        <v>1290285</v>
       </c>
       <c r="AC20">
-        <v>235457</v>
+        <v>139078</v>
       </c>
       <c r="AD20">
-        <v>1319020</v>
+        <v>712745</v>
       </c>
       <c r="AE20">
-        <v>59784</v>
+        <v>31051</v>
       </c>
       <c r="AF20">
-        <v>199223</v>
+        <v>121040</v>
       </c>
       <c r="AG20">
-        <v>244012</v>
+        <v>146052</v>
       </c>
       <c r="AH20">
-        <v>534404</v>
+        <v>321078</v>
       </c>
       <c r="AI20">
-        <v>174052</v>
+        <v>101108</v>
       </c>
       <c r="AJ20">
-        <v>2341718</v>
+        <v>1320088</v>
       </c>
       <c r="AK20">
-        <v>360511</v>
+        <v>198500</v>
       </c>
       <c r="AL20">
-        <v>1490333</v>
+        <v>813906</v>
       </c>
       <c r="AM20" t="s">
         <v>1</v>
@@ -3507,115 +3532,115 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>1211335</v>
+        <v>678548</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>489666</v>
+        <v>284466</v>
       </c>
       <c r="E21">
-        <v>2875</v>
+        <v>1224</v>
       </c>
       <c r="F21">
-        <v>23592</v>
+        <v>16640</v>
       </c>
       <c r="G21">
         <v>6</v>
       </c>
       <c r="H21">
-        <v>784349</v>
+        <v>379976</v>
       </c>
       <c r="I21">
-        <v>166527</v>
+        <v>83196</v>
       </c>
       <c r="J21">
-        <v>169441</v>
+        <v>103503</v>
       </c>
       <c r="K21">
-        <v>471285</v>
+        <v>260332</v>
       </c>
       <c r="L21">
-        <v>195265</v>
+        <v>99008</v>
       </c>
       <c r="M21">
-        <v>401647</v>
+        <v>189416</v>
       </c>
       <c r="N21">
-        <v>1176991</v>
+        <v>649708</v>
       </c>
       <c r="O21">
-        <v>611482</v>
+        <v>321982</v>
       </c>
       <c r="P21">
-        <v>616880</v>
+        <v>345958</v>
       </c>
       <c r="Q21">
-        <v>628609</v>
+        <v>376950</v>
       </c>
       <c r="R21">
-        <v>1017265</v>
+        <v>340529</v>
       </c>
       <c r="S21">
-        <v>607266</v>
+        <v>177728</v>
       </c>
       <c r="T21">
-        <v>314998</v>
+        <v>152460</v>
       </c>
       <c r="U21">
-        <v>1211335</v>
+        <v>119776</v>
       </c>
       <c r="V21">
-        <v>1211335</v>
+        <v>678548</v>
       </c>
       <c r="W21">
-        <v>555003</v>
+        <v>22216</v>
       </c>
       <c r="X21">
-        <v>627827</v>
+        <v>348798</v>
       </c>
       <c r="Y21">
-        <v>480045</v>
+        <v>259556</v>
       </c>
       <c r="Z21">
-        <v>938984</v>
+        <v>522303</v>
       </c>
       <c r="AA21">
-        <v>1209322</v>
+        <v>676980</v>
       </c>
       <c r="AB21">
-        <v>1185836</v>
+        <v>660559</v>
       </c>
       <c r="AC21">
-        <v>110162</v>
+        <v>63822</v>
       </c>
       <c r="AD21">
-        <v>717814</v>
+        <v>386906</v>
       </c>
       <c r="AE21">
-        <v>36333</v>
+        <v>18037</v>
       </c>
       <c r="AF21">
-        <v>88740</v>
+        <v>54636</v>
       </c>
       <c r="AG21">
-        <v>115945</v>
+        <v>66938</v>
       </c>
       <c r="AH21">
-        <v>265179</v>
+        <v>157736</v>
       </c>
       <c r="AI21">
-        <v>90928</v>
+        <v>51344</v>
       </c>
       <c r="AJ21">
-        <v>1205091</v>
+        <v>673640</v>
       </c>
       <c r="AK21">
-        <v>197067</v>
+        <v>103496</v>
       </c>
       <c r="AL21">
-        <v>801714</v>
+        <v>428732</v>
       </c>
       <c r="AM21" t="s">
         <v>1</v>
@@ -3674,19 +3699,19 @@
         <v>263418</v>
       </c>
       <c r="R22">
-        <v>473324</v>
+        <v>227822</v>
       </c>
       <c r="S22">
-        <v>303334</v>
+        <v>135906</v>
       </c>
       <c r="T22">
         <v>177210</v>
       </c>
       <c r="U22">
-        <v>555003</v>
+        <v>63926</v>
       </c>
       <c r="V22">
-        <v>555003</v>
+        <v>22216</v>
       </c>
       <c r="W22">
         <v>555003</v>
@@ -3793,19 +3818,19 @@
         <v>939190</v>
       </c>
       <c r="R23">
-        <v>1561620</v>
+        <v>1007313</v>
       </c>
       <c r="S23">
-        <v>757029</v>
+        <v>461769</v>
       </c>
       <c r="T23">
         <v>311865</v>
       </c>
       <c r="U23">
-        <v>1215681</v>
+        <v>683599</v>
       </c>
       <c r="V23">
-        <v>627827</v>
+        <v>348798</v>
       </c>
       <c r="W23">
         <v>290386</v>
@@ -3912,19 +3937,19 @@
         <v>622602</v>
       </c>
       <c r="R24">
-        <v>990650</v>
+        <v>598219</v>
       </c>
       <c r="S24">
-        <v>558395</v>
+        <v>309440</v>
       </c>
       <c r="T24">
         <v>269608</v>
       </c>
       <c r="U24">
-        <v>822933</v>
+        <v>427417</v>
       </c>
       <c r="V24">
-        <v>480045</v>
+        <v>259556</v>
       </c>
       <c r="W24">
         <v>233671</v>
@@ -4031,19 +4056,19 @@
         <v>1374422</v>
       </c>
       <c r="R25">
-        <v>2410002</v>
+        <v>1566512</v>
       </c>
       <c r="S25">
-        <v>1178570</v>
+        <v>714872</v>
       </c>
       <c r="T25">
         <v>491253</v>
       </c>
       <c r="U25">
-        <v>1832247</v>
+        <v>1037925</v>
       </c>
       <c r="V25">
-        <v>938984</v>
+        <v>522303</v>
       </c>
       <c r="W25">
         <v>433506</v>
@@ -4150,19 +4175,19 @@
         <v>1831115</v>
       </c>
       <c r="R26">
-        <v>3117552</v>
+        <v>1997856</v>
       </c>
       <c r="S26">
-        <v>1532092</v>
+        <v>921991</v>
       </c>
       <c r="T26">
         <v>644379</v>
       </c>
       <c r="U26">
-        <v>2357448</v>
+        <v>1331593</v>
       </c>
       <c r="V26">
-        <v>1209322</v>
+        <v>676980</v>
       </c>
       <c r="W26">
         <v>554548</v>
@@ -4269,19 +4294,19 @@
         <v>1716589</v>
       </c>
       <c r="R27">
-        <v>3020514</v>
+        <v>1923953</v>
       </c>
       <c r="S27">
-        <v>1506721</v>
+        <v>904541</v>
       </c>
       <c r="T27">
         <v>636346</v>
       </c>
       <c r="U27">
-        <v>2293942</v>
+        <v>1290285</v>
       </c>
       <c r="V27">
-        <v>1185836</v>
+        <v>660559</v>
       </c>
       <c r="W27">
         <v>547443</v>
@@ -4388,19 +4413,19 @@
         <v>209852</v>
       </c>
       <c r="R28">
-        <v>320235</v>
+        <v>208496</v>
       </c>
       <c r="S28">
-        <v>141217</v>
+        <v>89139</v>
       </c>
       <c r="T28">
         <v>53857</v>
       </c>
       <c r="U28">
-        <v>235457</v>
+        <v>139078</v>
       </c>
       <c r="V28">
-        <v>110162</v>
+        <v>63822</v>
       </c>
       <c r="W28">
         <v>47788</v>
@@ -4507,19 +4532,19 @@
         <v>935078</v>
       </c>
       <c r="R29">
-        <v>1682463</v>
+        <v>1036125</v>
       </c>
       <c r="S29">
-        <v>894078</v>
+        <v>516358</v>
       </c>
       <c r="T29">
         <v>399065</v>
       </c>
       <c r="U29">
-        <v>1319020</v>
+        <v>712745</v>
       </c>
       <c r="V29">
-        <v>717814</v>
+        <v>386906</v>
       </c>
       <c r="W29">
         <v>344496</v>
@@ -4626,19 +4651,19 @@
         <v>33776</v>
       </c>
       <c r="R30">
-        <v>74040</v>
+        <v>46798</v>
       </c>
       <c r="S30">
-        <v>43868</v>
+        <v>24570</v>
       </c>
       <c r="T30">
         <v>21371</v>
       </c>
       <c r="U30">
-        <v>59784</v>
+        <v>31051</v>
       </c>
       <c r="V30">
-        <v>36333</v>
+        <v>18037</v>
       </c>
       <c r="W30">
         <v>19435</v>
@@ -4745,19 +4770,19 @@
         <v>185889</v>
       </c>
       <c r="R31">
-        <v>281320</v>
+        <v>194214</v>
       </c>
       <c r="S31">
-        <v>114615</v>
+        <v>76772</v>
       </c>
       <c r="T31">
         <v>39458</v>
       </c>
       <c r="U31">
-        <v>199223</v>
+        <v>121040</v>
       </c>
       <c r="V31">
-        <v>88740</v>
+        <v>54636</v>
       </c>
       <c r="W31">
         <v>35081</v>
@@ -4864,19 +4889,19 @@
         <v>203556</v>
       </c>
       <c r="R32">
-        <v>324637</v>
+        <v>215385</v>
       </c>
       <c r="S32">
-        <v>144673</v>
+        <v>93109</v>
       </c>
       <c r="T32">
         <v>53309</v>
       </c>
       <c r="U32">
-        <v>244012</v>
+        <v>146052</v>
       </c>
       <c r="V32">
-        <v>115945</v>
+        <v>66938</v>
       </c>
       <c r="W32">
         <v>50623</v>
@@ -4983,19 +5008,19 @@
         <v>273782</v>
       </c>
       <c r="R33">
-        <v>558086</v>
+        <v>391650</v>
       </c>
       <c r="S33">
-        <v>204239</v>
+        <v>146380</v>
       </c>
       <c r="T33">
         <v>58587</v>
       </c>
       <c r="U33">
-        <v>534404</v>
+        <v>321078</v>
       </c>
       <c r="V33">
-        <v>265179</v>
+        <v>157736</v>
       </c>
       <c r="W33">
         <v>112437</v>
@@ -5102,19 +5127,19 @@
         <v>74632</v>
       </c>
       <c r="R34">
-        <v>161184</v>
+        <v>113904</v>
       </c>
       <c r="S34">
-        <v>53904</v>
+        <v>39096</v>
       </c>
       <c r="T34">
         <v>14808</v>
       </c>
       <c r="U34">
-        <v>174052</v>
+        <v>101108</v>
       </c>
       <c r="V34">
-        <v>90928</v>
+        <v>51344</v>
       </c>
       <c r="W34">
         <v>41472</v>
@@ -5221,19 +5246,19 @@
         <v>1796090</v>
       </c>
       <c r="R35">
-        <v>3093580</v>
+        <v>1979168</v>
       </c>
       <c r="S35">
-        <v>1527193</v>
+        <v>918168</v>
       </c>
       <c r="T35">
         <v>643321</v>
       </c>
       <c r="U35">
-        <v>2341718</v>
+        <v>1320088</v>
       </c>
       <c r="V35">
-        <v>1205091</v>
+        <v>673640</v>
       </c>
       <c r="W35">
         <v>553667</v>
@@ -5340,19 +5365,19 @@
         <v>0</v>
       </c>
       <c r="R36">
-        <v>412684</v>
+        <v>245594</v>
       </c>
       <c r="S36">
-        <v>202422</v>
+        <v>121208</v>
       </c>
       <c r="T36">
         <v>84087</v>
       </c>
       <c r="U36">
-        <v>360511</v>
+        <v>198500</v>
       </c>
       <c r="V36">
-        <v>197067</v>
+        <v>103496</v>
       </c>
       <c r="W36">
         <v>98950</v>
@@ -5459,19 +5484,19 @@
         <v>1063414</v>
       </c>
       <c r="R37">
-        <v>1947504</v>
+        <v>1227495</v>
       </c>
       <c r="S37">
-        <v>1010038</v>
+        <v>592239</v>
       </c>
       <c r="T37">
         <v>441651</v>
       </c>
       <c r="U37">
-        <v>1490333</v>
+        <v>813906</v>
       </c>
       <c r="V37">
-        <v>801714</v>
+        <v>428732</v>
       </c>
       <c r="W37">
         <v>388191</v>
@@ -5534,8 +5559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:G45"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5711,19 +5736,19 @@
         <v>1838655</v>
       </c>
       <c r="R2" s="3">
-        <v>3131464</v>
+        <v>2007816</v>
       </c>
       <c r="S2" s="3">
-        <v>1537082</v>
+        <v>925730</v>
       </c>
       <c r="T2" s="3">
         <v>645648</v>
       </c>
       <c r="U2" s="3">
-        <v>2364652</v>
+        <v>1336971</v>
       </c>
       <c r="V2" s="3">
-        <v>1211335</v>
+        <v>678548</v>
       </c>
       <c r="W2" s="3">
         <v>555003</v>
@@ -5995,11 +6020,11 @@
       </c>
       <c r="R4" s="3">
         <f>'cf1-cor'!R3/$B4</f>
-        <v>0.7085453398120809</v>
+        <v>0.47028721742838997</v>
       </c>
       <c r="S4" s="3">
         <f>'cf1-cor'!S3/$B4</f>
-        <v>0.30820722037389503</v>
+        <v>0.19738668243057353</v>
       </c>
       <c r="T4" s="3">
         <f>'cf1-cor'!T3/$B4</f>
@@ -6007,11 +6032,11 @@
       </c>
       <c r="U4" s="3">
         <f>'cf1-cor'!U3/$B4</f>
-        <v>0.52305369103492572</v>
+        <v>0.30625070952922034</v>
       </c>
       <c r="V4" s="3">
         <f>'cf1-cor'!V3/$B4</f>
-        <v>0.25040168302887922</v>
+        <v>0.14546806428155756</v>
       </c>
       <c r="W4" s="3">
         <f>'cf1-cor'!W3/$B4</f>
@@ -6147,11 +6172,11 @@
       </c>
       <c r="R5" s="3">
         <f>'cf1-cor'!R4/$B5</f>
-        <v>0.58139435047651755</v>
+        <v>0.40418133424916286</v>
       </c>
       <c r="S5" s="3">
         <f>'cf1-cor'!S4/$B5</f>
-        <v>0.20533184511032884</v>
+        <v>0.12715720786468618</v>
       </c>
       <c r="T5" s="3">
         <f>'cf1-cor'!T4/$B5</f>
@@ -6159,11 +6184,11 @@
       </c>
       <c r="U5" s="3">
         <f>'cf1-cor'!U4/$B5</f>
-        <v>0.4063707392461578</v>
+        <v>0.28792822185970635</v>
       </c>
       <c r="V5" s="3">
         <f>'cf1-cor'!V4/$B5</f>
-        <v>0.1234223405168713</v>
+        <v>5.2545719927878425E-2</v>
       </c>
       <c r="W5" s="3">
         <f>'cf1-cor'!W4/$B5</f>
@@ -6299,11 +6324,11 @@
       </c>
       <c r="R6" s="3">
         <f>'cf1-cor'!R5/$B6</f>
-        <v>0.48591929419647845</v>
+        <v>0.36744313740088597</v>
       </c>
       <c r="S6" s="3">
         <f>'cf1-cor'!S5/$B6</f>
-        <v>0.13317109034731786</v>
+        <v>9.3786062614004392E-2</v>
       </c>
       <c r="T6" s="3">
         <f>'cf1-cor'!T5/$B6</f>
@@ -6311,11 +6336,11 @@
       </c>
       <c r="U6" s="3">
         <f>'cf1-cor'!U5/$B6</f>
-        <v>0.30773740833116181</v>
+        <v>0.20461694524066559</v>
       </c>
       <c r="V6" s="3">
         <f>'cf1-cor'!V5/$B6</f>
-        <v>0.10977925026988795</v>
+        <v>7.7429922197818565E-2</v>
       </c>
       <c r="W6" s="3">
         <f>'cf1-cor'!W5/$B6</f>
@@ -6451,7 +6476,7 @@
       </c>
       <c r="R7" s="3">
         <f>'cf1-cor'!R6/$B7</f>
-        <v>0.13043478260869565</v>
+        <v>6.5217391304347824E-2</v>
       </c>
       <c r="S7" s="3">
         <f>'cf1-cor'!S6/$B7</f>
@@ -6463,7 +6488,7 @@
       </c>
       <c r="U7" s="3">
         <f>'cf1-cor'!U6/$B7</f>
-        <v>0.17391304347826086</v>
+        <v>0.10869565217391304</v>
       </c>
       <c r="V7" s="3">
         <f>'cf1-cor'!V6/$B7</f>
@@ -6603,11 +6628,11 @@
       </c>
       <c r="R8" s="3">
         <f>'cf1-cor'!R7/$B8</f>
-        <v>0.85550275695771216</v>
+        <v>0.49194249851674043</v>
       </c>
       <c r="S8" s="3">
         <f>'cf1-cor'!S7/$B8</f>
-        <v>0.50896868553263985</v>
+        <v>0.26411382724516513</v>
       </c>
       <c r="T8" s="3">
         <f>'cf1-cor'!T7/$B8</f>
@@ -6615,11 +6640,11 @@
       </c>
       <c r="U8" s="3">
         <f>'cf1-cor'!U7/$B8</f>
-        <v>0.69898430738581618</v>
+        <v>0.33981667455924058</v>
       </c>
       <c r="V8" s="3">
         <f>'cf1-cor'!V7/$B8</f>
-        <v>0.42693327237000389</v>
+        <v>0.20682680426961034</v>
       </c>
       <c r="W8" s="3">
         <f>'cf1-cor'!W7/$B8</f>
@@ -6755,11 +6780,11 @@
       </c>
       <c r="R9" s="3">
         <f>'cf1-cor'!R8/$B9</f>
-        <v>0.82239719417178636</v>
+        <v>0.47882917873031566</v>
       </c>
       <c r="S9" s="3">
         <f>'cf1-cor'!S8/$B9</f>
-        <v>0.47314219805569285</v>
+        <v>0.2799778735023421</v>
       </c>
       <c r="T9" s="3">
         <f>'cf1-cor'!T8/$B9</f>
@@ -6767,11 +6792,11 @@
       </c>
       <c r="U9" s="3">
         <f>'cf1-cor'!U8/$B9</f>
-        <v>0.69963750205964736</v>
+        <v>0.37358237412612105</v>
       </c>
       <c r="V9" s="3">
         <f>'cf1-cor'!V8/$B9</f>
-        <v>0.39198502930584</v>
+        <v>0.19583362756867453</v>
       </c>
       <c r="W9" s="3">
         <f>'cf1-cor'!W8/$B9</f>
@@ -6907,11 +6932,11 @@
       </c>
       <c r="R10" s="3">
         <f>'cf1-cor'!R9/$B10</f>
-        <v>0.69856454330533824</v>
+        <v>0.47886391243583548</v>
       </c>
       <c r="S10" s="3">
         <f>'cf1-cor'!S9/$B10</f>
-        <v>0.28614568775224986</v>
+        <v>0.18987604655111609</v>
       </c>
       <c r="T10" s="3">
         <f>'cf1-cor'!T9/$B10</f>
@@ -6919,11 +6944,11 @@
       </c>
       <c r="U10" s="3">
         <f>'cf1-cor'!U9/$B10</f>
-        <v>0.49621478298350336</v>
+        <v>0.30206763234545003</v>
       </c>
       <c r="V10" s="3">
         <f>'cf1-cor'!V9/$B10</f>
-        <v>0.22131502984548268</v>
+        <v>0.13519024046185393</v>
       </c>
       <c r="W10" s="3">
         <f>'cf1-cor'!W9/$B10</f>
@@ -7059,11 +7084,11 @@
       </c>
       <c r="R11" s="3">
         <f>'cf1-cor'!R10/$B11</f>
-        <v>0.87736079241639242</v>
+        <v>0.53188129674429552</v>
       </c>
       <c r="S11" s="3">
         <f>'cf1-cor'!S10/$B11</f>
-        <v>0.49392259265796584</v>
+        <v>0.27498710800549597</v>
       </c>
       <c r="T11" s="3">
         <f>'cf1-cor'!T10/$B11</f>
@@ -7071,11 +7096,11 @@
       </c>
       <c r="U11" s="3">
         <f>'cf1-cor'!U10/$B11</f>
-        <v>0.71111895590418739</v>
+        <v>0.3735701999383953</v>
       </c>
       <c r="V11" s="3">
         <f>'cf1-cor'!V10/$B11</f>
-        <v>0.40777205569341624</v>
+        <v>0.22524823578679237</v>
       </c>
       <c r="W11" s="3">
         <f>'cf1-cor'!W10/$B11</f>
@@ -7211,11 +7236,11 @@
       </c>
       <c r="R12" s="3">
         <f>'cf1-cor'!R11/$B12</f>
-        <v>0.76764026845637579</v>
+        <v>0.29677852348993289</v>
       </c>
       <c r="S12" s="3">
         <f>'cf1-cor'!S11/$B12</f>
-        <v>0.60042953020134227</v>
+        <v>0.30371543624161074</v>
       </c>
       <c r="T12" s="3">
         <f>'cf1-cor'!T11/$B12</f>
@@ -7223,11 +7248,11 @@
       </c>
       <c r="U12" s="3">
         <f>'cf1-cor'!U11/$B12</f>
-        <v>0.80319463087248322</v>
+        <v>0.38644563758389261</v>
       </c>
       <c r="V12" s="3">
         <f>'cf1-cor'!V11/$B12</f>
-        <v>0.5242013422818792</v>
+        <v>0.26579328859060403</v>
       </c>
       <c r="W12" s="3">
         <f>'cf1-cor'!W11/$B12</f>
@@ -7363,11 +7388,11 @@
       </c>
       <c r="R13" s="3">
         <f>'cf1-cor'!R12/$B13</f>
-        <v>0.74253712601918664</v>
+        <v>0.41864295400894036</v>
       </c>
       <c r="S13" s="3">
         <f>'cf1-cor'!S12/$B13</f>
-        <v>0.41674479733462805</v>
+        <v>0.20978502904786619</v>
       </c>
       <c r="T13" s="3">
         <f>'cf1-cor'!T12/$B13</f>
@@ -7375,11 +7400,11 @@
       </c>
       <c r="U13" s="3">
         <f>'cf1-cor'!U12/$B13</f>
-        <v>0.67284945336436242</v>
+        <v>0.30840441828927323</v>
       </c>
       <c r="V13" s="3">
         <f>'cf1-cor'!V12/$B13</f>
-        <v>0.42028055885750643</v>
+        <v>0.19820355271308746</v>
       </c>
       <c r="W13" s="3">
         <f>'cf1-cor'!W12/$B13</f>
@@ -7515,11 +7540,11 @@
       </c>
       <c r="R14" s="3">
         <f>'cf1-cor'!R13/$B14</f>
-        <v>0.76809452851176363</v>
+        <v>0.48694146535983379</v>
       </c>
       <c r="S14" s="3">
         <f>'cf1-cor'!S13/$B14</f>
-        <v>0.38262797238021279</v>
+        <v>0.22753426238797825</v>
       </c>
       <c r="T14" s="3">
         <f>'cf1-cor'!T13/$B14</f>
@@ -7527,11 +7552,11 @@
       </c>
       <c r="U14" s="3">
         <f>'cf1-cor'!U13/$B14</f>
-        <v>0.58954183894054191</v>
+        <v>0.32782625348920186</v>
       </c>
       <c r="V14" s="3">
         <f>'cf1-cor'!V13/$B14</f>
-        <v>0.3087788842949189</v>
+        <v>0.17044829684974919</v>
       </c>
       <c r="W14" s="3">
         <f>'cf1-cor'!W13/$B14</f>
@@ -7667,11 +7692,11 @@
       </c>
       <c r="R15" s="3">
         <f>'cf1-cor'!R14/$B15</f>
-        <v>0.76648978863818784</v>
+        <v>0.47416949076964238</v>
       </c>
       <c r="S15" s="3">
         <f>'cf1-cor'!S14/$B15</f>
-        <v>0.39604699901899582</v>
+        <v>0.22664652635333987</v>
       </c>
       <c r="T15" s="3">
         <f>'cf1-cor'!T14/$B15</f>
@@ -7679,11 +7704,11 @@
       </c>
       <c r="U15" s="3">
         <f>'cf1-cor'!U14/$B15</f>
-        <v>0.61668766164273614</v>
+        <v>0.32893014804245074</v>
       </c>
       <c r="V15" s="3">
         <f>'cf1-cor'!V14/$B15</f>
-        <v>0.34083318469633461</v>
+        <v>0.17946914295906538</v>
       </c>
       <c r="W15" s="3">
         <f>'cf1-cor'!W14/$B15</f>
@@ -7819,11 +7844,11 @@
       </c>
       <c r="R16" s="3">
         <f>'cf1-cor'!R15/$B16</f>
-        <v>0.79322941433682692</v>
+        <v>0.52908809470588047</v>
       </c>
       <c r="S16" s="3">
         <f>'cf1-cor'!S15/$B16</f>
-        <v>0.39099541879716476</v>
+        <v>0.23946059684901724</v>
       </c>
       <c r="T16" s="3">
         <f>'cf1-cor'!T15/$B16</f>
@@ -7831,11 +7856,11 @@
       </c>
       <c r="U16" s="3">
         <f>'cf1-cor'!U15/$B16</f>
-        <v>0.57570977844375371</v>
+        <v>0.33134504992563768</v>
       </c>
       <c r="V16" s="3">
         <f>'cf1-cor'!V15/$B16</f>
-        <v>0.28787332229837598</v>
+        <v>0.16144481720221365</v>
       </c>
       <c r="W16" s="3">
         <f>'cf1-cor'!W15/$B16</f>
@@ -7971,11 +7996,11 @@
       </c>
       <c r="R17" s="3">
         <f>'cf1-cor'!R16/$B17</f>
-        <v>0.78125531978538665</v>
+        <v>0.50084763046901126</v>
       </c>
       <c r="S17" s="3">
         <f>'cf1-cor'!S16/$B17</f>
-        <v>0.39052731480348407</v>
+        <v>0.23162692294095413</v>
       </c>
       <c r="T17" s="3">
         <f>'cf1-cor'!T16/$B17</f>
@@ -7983,11 +8008,11 @@
       </c>
       <c r="U17" s="3">
         <f>'cf1-cor'!U16/$B17</f>
-        <v>0.62895921203270866</v>
+        <v>0.33933445915628546</v>
       </c>
       <c r="V17" s="3">
         <f>'cf1-cor'!V16/$B17</f>
-        <v>0.34188523676274235</v>
+        <v>0.20501399120552796</v>
       </c>
       <c r="W17" s="3">
         <f>'cf1-cor'!W16/$B17</f>
@@ -8059,7 +8084,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>3131464</v>
+        <v>2007816</v>
       </c>
       <c r="C18" s="3">
         <f>'cf1-cor'!C17/$B18</f>
@@ -8067,59 +8092,59 @@
       </c>
       <c r="D18" s="3">
         <f>'cf1-cor'!D17/$B18</f>
-        <v>0.44246908155418679</v>
+        <v>0.45803848559828192</v>
       </c>
       <c r="E18" s="3">
         <f>'cf1-cor'!E17/$B18</f>
-        <v>4.3248142083064023E-3</v>
+        <v>4.6891747052518759E-3</v>
       </c>
       <c r="F18" s="3">
         <f>'cf1-cor'!F17/$B18</f>
-        <v>3.3347341690659706E-2</v>
+        <v>3.9328803037728559E-2</v>
       </c>
       <c r="G18" s="3">
         <f>'cf1-cor'!G17/$B18</f>
-        <v>3.832073432745834E-6</v>
+        <v>2.9883216390346526E-6</v>
       </c>
       <c r="H18" s="3">
         <f>'cf1-cor'!H17/$B18</f>
-        <v>0.50190709521169652</v>
+        <v>0.45013188459500275</v>
       </c>
       <c r="I18" s="3">
         <f>'cf1-cor'!I17/$B18</f>
-        <v>0.11157049865494223</v>
+        <v>0.10131456268901134</v>
       </c>
       <c r="J18" s="3">
         <f>'cf1-cor'!J17/$B18</f>
-        <v>0.17079168082404908</v>
+        <v>0.18259790737796691</v>
       </c>
       <c r="K18" s="3">
         <f>'cf1-cor'!K17/$B18</f>
-        <v>0.3238149951588139</v>
+        <v>0.3061660032592628</v>
       </c>
       <c r="L18" s="3">
         <f>'cf1-cor'!L17/$B18</f>
-        <v>9.1313839149995024E-2</v>
+        <v>5.5059826199213471E-2</v>
       </c>
       <c r="M18" s="3">
         <f>'cf1-cor'!M17/$B18</f>
-        <v>0.22660838508761397</v>
+        <v>0.19926228299804363</v>
       </c>
       <c r="N18" s="3">
         <f>'cf1-cor'!N17/$B18</f>
-        <v>0.93495949498381592</v>
+        <v>0.92443929124979585</v>
       </c>
       <c r="O18" s="3">
         <f>'cf1-cor'!O17/$B18</f>
-        <v>0.43913773238331977</v>
+        <v>0.42369320694725016</v>
       </c>
       <c r="P18" s="3">
         <f>'cf1-cor'!P17/$B18</f>
-        <v>0.54281352108790015</v>
+        <v>0.56468122576969204</v>
       </c>
       <c r="Q18" s="3">
         <f>'cf1-cor'!Q17/$B18</f>
-        <v>0.45871803092738733</v>
+        <v>0.45865059348067749</v>
       </c>
       <c r="R18" s="3">
         <f>'cf1-cor'!R17/$B18</f>
@@ -8127,83 +8152,83 @@
       </c>
       <c r="S18" s="3">
         <f>'cf1-cor'!S17/$B18</f>
-        <v>0.49085092467931934</v>
+        <v>0.13016332173864537</v>
       </c>
       <c r="T18" s="3">
         <f>'cf1-cor'!T17/$B18</f>
-        <v>0.20618087897545684</v>
+        <v>7.6948286097929294E-2</v>
       </c>
       <c r="U18" s="3">
         <f>'cf1-cor'!U17/$B18</f>
-        <v>0.61025577812805765</v>
+        <v>0.31661217960211496</v>
       </c>
       <c r="V18" s="3">
         <f>'cf1-cor'!V17/$B18</f>
-        <v>0.32485284838018258</v>
+        <v>0.1696016965698052</v>
       </c>
       <c r="W18" s="3">
         <f>'cf1-cor'!W17/$B18</f>
-        <v>0.15115102712341574</v>
+        <v>0.11346756874135877</v>
       </c>
       <c r="X18" s="3">
         <f>'cf1-cor'!X17/$B18</f>
-        <v>0.4986868761703791</v>
+        <v>0.50169587253015213</v>
       </c>
       <c r="Y18" s="3">
         <f>'cf1-cor'!Y17/$B18</f>
-        <v>0.31635362884580503</v>
+        <v>0.29794513043027848</v>
       </c>
       <c r="Z18" s="3">
         <f>'cf1-cor'!Z17/$B18</f>
-        <v>0.76960871975536038</v>
+        <v>0.78020695123457529</v>
       </c>
       <c r="AA18" s="3">
         <f>'cf1-cor'!AA17/$B18</f>
-        <v>0.99555734953363662</v>
+        <v>0.9950393860792025</v>
       </c>
       <c r="AB18" s="3">
         <f>'cf1-cor'!AB17/$B18</f>
-        <v>0.96456928771973749</v>
+        <v>0.95823173039760612</v>
       </c>
       <c r="AC18" s="3">
         <f>'cf1-cor'!AC17/$B18</f>
-        <v>0.1022636696446135</v>
+        <v>0.10384218474202815</v>
       </c>
       <c r="AD18" s="3">
         <f>'cf1-cor'!AD17/$B18</f>
-        <v>0.53727681365648783</v>
+        <v>0.51604579304079656</v>
       </c>
       <c r="AE18" s="3">
         <f>'cf1-cor'!AE17/$B18</f>
-        <v>2.3643893080041795E-2</v>
+        <v>2.3307912677257278E-2</v>
       </c>
       <c r="AF18" s="3">
         <f>'cf1-cor'!AF17/$B18</f>
-        <v>8.9836574841671499E-2</v>
+        <v>9.6728983133912663E-2</v>
       </c>
       <c r="AG18" s="3">
         <f>'cf1-cor'!AG17/$B18</f>
-        <v>0.10366940191552577</v>
+        <v>0.10727327603724644</v>
       </c>
       <c r="AH18" s="3">
         <f>'cf1-cor'!AH17/$B18</f>
-        <v>0.17821887781561596</v>
+        <v>0.19506269498798695</v>
       </c>
       <c r="AI18" s="3">
         <f>'cf1-cor'!AI17/$B18</f>
-        <v>5.1472410348642042E-2</v>
+        <v>5.6730297995433845E-2</v>
       </c>
       <c r="AJ18" s="3">
         <f>'cf1-cor'!AJ17/$B18</f>
-        <v>0.98790214417282141</v>
+        <v>0.98573176028082254</v>
       </c>
       <c r="AK18" s="3">
         <f>'cf1-cor'!AK17/$B18</f>
-        <v>0.13178628270994014</v>
+        <v>0.12231897743617941</v>
       </c>
       <c r="AL18" s="3">
         <f>'cf1-cor'!AL17/$B18</f>
-        <v>0.62191486154718689</v>
+        <v>0.61135831171780686</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
@@ -8211,7 +8236,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>1537082</v>
+        <v>925730</v>
       </c>
       <c r="C19" s="3">
         <f>'cf1-cor'!C18/$B19</f>
@@ -8219,63 +8244,63 @@
       </c>
       <c r="D19" s="3">
         <f>'cf1-cor'!D18/$B19</f>
-        <v>0.39211050549027315</v>
+        <v>0.41696174910611083</v>
       </c>
       <c r="E19" s="3">
         <f>'cf1-cor'!E18/$B19</f>
-        <v>3.1117402975247904E-3</v>
+        <v>3.1996370431983407E-3</v>
       </c>
       <c r="F19" s="3">
         <f>'cf1-cor'!F18/$B19</f>
-        <v>1.8619045698277645E-2</v>
+        <v>2.1772006956672033E-2</v>
       </c>
       <c r="G19" s="3">
         <f>'cf1-cor'!G18/$B19</f>
-        <v>3.9035002686909355E-6</v>
+        <v>6.4813714582005553E-6</v>
       </c>
       <c r="H19" s="3">
         <f>'cf1-cor'!H18/$B19</f>
-        <v>0.60833579470711385</v>
+        <v>0.5241506702818316</v>
       </c>
       <c r="I19" s="3">
         <f>'cf1-cor'!I18/$B19</f>
-        <v>0.1307705119180369</v>
+        <v>0.12848562755879145</v>
       </c>
       <c r="J19" s="3">
         <f>'cf1-cor'!J18/$B19</f>
-        <v>0.14252720414395589</v>
+        <v>0.15703390837501216</v>
       </c>
       <c r="K19" s="3">
         <f>'cf1-cor'!K18/$B19</f>
-        <v>0.37138812373054919</v>
+        <v>0.34331608568373068</v>
       </c>
       <c r="L19" s="3">
         <f>'cf1-cor'!L18/$B19</f>
-        <v>0.14550947834923575</v>
+        <v>0.12221057975867694</v>
       </c>
       <c r="M19" s="3">
         <f>'cf1-cor'!M18/$B19</f>
-        <v>0.25910654083516688</v>
+        <v>0.21656854590431335</v>
       </c>
       <c r="N19" s="3">
         <f>'cf1-cor'!N18/$B19</f>
-        <v>0.94886674881366118</v>
+        <v>0.93688872565434844</v>
       </c>
       <c r="O19" s="3">
         <f>'cf1-cor'!O18/$B19</f>
-        <v>0.46226551348594286</v>
+        <v>0.43924470417940437</v>
       </c>
       <c r="P19" s="3">
         <f>'cf1-cor'!P18/$B19</f>
-        <v>0.5450971386041864</v>
+        <v>0.55430525099110972</v>
       </c>
       <c r="Q19" s="3">
         <f>'cf1-cor'!Q18/$B19</f>
-        <v>0.46714814173869706</v>
+        <v>0.46004990656022815</v>
       </c>
       <c r="R19" s="3">
         <f>'cf1-cor'!R18/$B19</f>
-        <v>1</v>
+        <v>0.28231125706199434</v>
       </c>
       <c r="S19" s="3">
         <f>'cf1-cor'!S18/$B19</f>
@@ -8283,79 +8308,79 @@
       </c>
       <c r="T19" s="3">
         <f>'cf1-cor'!T18/$B19</f>
-        <v>0.42004785691329416</v>
+        <v>3.7047519255074372E-2</v>
       </c>
       <c r="U19" s="3">
         <f>'cf1-cor'!U18/$B19</f>
-        <v>0.6861091340605121</v>
+        <v>0.40430147019109242</v>
       </c>
       <c r="V19" s="3">
         <f>'cf1-cor'!V18/$B19</f>
-        <v>0.39507716569447826</v>
+        <v>0.19198686442051138</v>
       </c>
       <c r="W19" s="3">
         <f>'cf1-cor'!W18/$B19</f>
-        <v>0.19734405841718269</v>
+        <v>0.14680954489970077</v>
       </c>
       <c r="X19" s="3">
         <f>'cf1-cor'!X18/$B19</f>
-        <v>0.49251048415113835</v>
+        <v>0.49881606948030205</v>
       </c>
       <c r="Y19" s="3">
         <f>'cf1-cor'!Y18/$B19</f>
-        <v>0.36328250542261248</v>
+        <v>0.33426593067092997</v>
       </c>
       <c r="Z19" s="3">
         <f>'cf1-cor'!Z18/$B19</f>
-        <v>0.76675805194517921</v>
+        <v>0.77222516284445786</v>
       </c>
       <c r="AA19" s="3">
         <f>'cf1-cor'!AA18/$B19</f>
-        <v>0.99675358894320543</v>
+        <v>0.99596102535296471</v>
       </c>
       <c r="AB19" s="3">
         <f>'cf1-cor'!AB18/$B19</f>
-        <v>0.98024763805704573</v>
+        <v>0.9771110366953647</v>
       </c>
       <c r="AC19" s="3">
         <f>'cf1-cor'!AC18/$B19</f>
-        <v>9.1873432907287972E-2</v>
+        <v>9.6290495068756546E-2</v>
       </c>
       <c r="AD19" s="3">
         <f>'cf1-cor'!AD18/$B19</f>
-        <v>0.5816722855384423</v>
+        <v>0.55778466723558706</v>
       </c>
       <c r="AE19" s="3">
         <f>'cf1-cor'!AE18/$B19</f>
-        <v>2.8539791631155657E-2</v>
+        <v>2.6541216121331274E-2</v>
       </c>
       <c r="AF19" s="3">
         <f>'cf1-cor'!AF18/$B19</f>
-        <v>7.4566613882668595E-2</v>
+        <v>8.2931308264828835E-2</v>
       </c>
       <c r="AG19" s="3">
         <f>'cf1-cor'!AG18/$B19</f>
-        <v>9.4121849062053939E-2</v>
+        <v>0.10057900251693258</v>
       </c>
       <c r="AH19" s="3">
         <f>'cf1-cor'!AH18/$B19</f>
-        <v>0.13287449856286132</v>
+        <v>0.15812385900856621</v>
       </c>
       <c r="AI19" s="3">
         <f>'cf1-cor'!AI18/$B19</f>
-        <v>3.5069046413919364E-2</v>
+        <v>4.2232616421634818E-2</v>
       </c>
       <c r="AJ19" s="3">
         <f>'cf1-cor'!AJ18/$B19</f>
-        <v>0.99356638097381922</v>
+        <v>0.99183131150551451</v>
       </c>
       <c r="AK19" s="3">
         <f>'cf1-cor'!AK18/$B19</f>
-        <v>0.13169238856482607</v>
+        <v>0.13093234528426215</v>
       </c>
       <c r="AL19" s="3">
         <f>'cf1-cor'!AL18/$B19</f>
-        <v>0.65711393406467578</v>
+        <v>0.63975349183887309</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
@@ -8427,11 +8452,11 @@
       </c>
       <c r="R20" s="3">
         <f>'cf1-cor'!R19/$B20</f>
-        <v>1</v>
+        <v>0.23929137858399624</v>
       </c>
       <c r="S20" s="3">
         <f>'cf1-cor'!S19/$B20</f>
-        <v>1</v>
+        <v>5.3118727232176047E-2</v>
       </c>
       <c r="T20" s="3">
         <f>'cf1-cor'!T19/$B20</f>
@@ -8439,11 +8464,11 @@
       </c>
       <c r="U20" s="3">
         <f>'cf1-cor'!U19/$B20</f>
-        <v>0.7188963645825589</v>
+        <v>0.30904765444948329</v>
       </c>
       <c r="V20" s="3">
         <f>'cf1-cor'!V19/$B20</f>
-        <v>0.48787884419993555</v>
+        <v>0.23613485986172031</v>
       </c>
       <c r="W20" s="3">
         <f>'cf1-cor'!W19/$B20</f>
@@ -8515,7 +8540,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>2364652</v>
+        <v>1336971</v>
       </c>
       <c r="C21" s="3">
         <f>'cf1-cor'!C20/$B21</f>
@@ -8523,71 +8548,71 @@
       </c>
       <c r="D21" s="3">
         <f>'cf1-cor'!D20/$B21</f>
-        <v>0.432555403501234</v>
+        <v>0.44793791338779976</v>
       </c>
       <c r="E21" s="3">
         <f>'cf1-cor'!E20/$B21</f>
-        <v>4.0031260413794503E-3</v>
+        <v>5.0165635604661578E-3</v>
       </c>
       <c r="F21" s="3">
         <f>'cf1-cor'!F20/$B21</f>
-        <v>2.7967751702999005E-2</v>
+        <v>3.2890017808912833E-2</v>
       </c>
       <c r="G21" s="3">
         <f>'cf1-cor'!G20/$B21</f>
-        <v>6.7663233321435884E-6</v>
+        <v>7.4795937982200059E-6</v>
       </c>
       <c r="H21" s="3">
         <f>'cf1-cor'!H20/$B21</f>
-        <v>0.54306215037138661</v>
+        <v>0.4669517887822548</v>
       </c>
       <c r="I21" s="3">
         <f>'cf1-cor'!I20/$B21</f>
-        <v>0.12569587406519014</v>
+        <v>0.11870788521216989</v>
       </c>
       <c r="J21" s="3">
         <f>'cf1-cor'!J20/$B21</f>
-        <v>0.16066084988404214</v>
+        <v>0.1729775739339148</v>
       </c>
       <c r="K21" s="3">
         <f>'cf1-cor'!K20/$B21</f>
-        <v>0.34756911376388577</v>
+        <v>0.32293594999442771</v>
       </c>
       <c r="L21" s="3">
         <f>'cf1-cor'!L20/$B21</f>
-        <v>0.12652601735900251</v>
+        <v>0.10766950068475681</v>
       </c>
       <c r="M21" s="3">
         <f>'cf1-cor'!M20/$B21</f>
-        <v>0.27192923102426914</v>
+        <v>0.22044681597431806</v>
       </c>
       <c r="N21" s="3">
         <f>'cf1-cor'!N20/$B21</f>
-        <v>0.95032672883790092</v>
+        <v>0.93464630122867287</v>
       </c>
       <c r="O21" s="3">
         <f>'cf1-cor'!O20/$B21</f>
-        <v>0.46788576078002175</v>
+        <v>0.44139102493621779</v>
       </c>
       <c r="P21" s="3">
         <f>'cf1-cor'!P20/$B21</f>
-        <v>0.52171778342013964</v>
+        <v>0.53107733825191417</v>
       </c>
       <c r="Q21" s="3">
         <f>'cf1-cor'!Q20/$B21</f>
-        <v>0.48905251174379993</v>
+        <v>0.4666660682991628</v>
       </c>
       <c r="R21" s="3">
         <f>'cf1-cor'!R20/$B21</f>
-        <v>0.8081502056116503</v>
+        <v>0.47547702979346596</v>
       </c>
       <c r="S21" s="3">
         <f>'cf1-cor'!S20/$B21</f>
-        <v>0.44598782400116382</v>
+        <v>0.27994174892349949</v>
       </c>
       <c r="T21" s="3">
         <f>'cf1-cor'!T20/$B21</f>
-        <v>0.19628850249423593</v>
+        <v>0.14924482281216273</v>
       </c>
       <c r="U21" s="3">
         <f>'cf1-cor'!U20/$B21</f>
@@ -8595,71 +8620,71 @@
       </c>
       <c r="V21" s="3">
         <f>'cf1-cor'!V20/$B21</f>
-        <v>0.51226776709638455</v>
+        <v>8.9587582677559952E-2</v>
       </c>
       <c r="W21" s="3">
         <f>'cf1-cor'!W20/$B21</f>
-        <v>0.23470810926935548</v>
+        <v>4.7814051314501213E-2</v>
       </c>
       <c r="X21" s="3">
         <f>'cf1-cor'!X20/$B21</f>
-        <v>0.51410566967147808</v>
+        <v>0.51130428408693984</v>
       </c>
       <c r="Y21" s="3">
         <f>'cf1-cor'!Y20/$B21</f>
-        <v>0.34801442241818248</v>
+        <v>0.31969055424538007</v>
       </c>
       <c r="Z21" s="3">
         <f>'cf1-cor'!Z20/$B21</f>
-        <v>0.77484847664688083</v>
+        <v>0.77632573930174997</v>
       </c>
       <c r="AA21" s="3">
         <f>'cf1-cor'!AA20/$B21</f>
-        <v>0.99695346291970233</v>
+        <v>0.99597747445531726</v>
       </c>
       <c r="AB21" s="3">
         <f>'cf1-cor'!AB20/$B21</f>
-        <v>0.97009707982400795</v>
+        <v>0.96508076839363011</v>
       </c>
       <c r="AC21" s="3">
         <f>'cf1-cor'!AC20/$B21</f>
-        <v>9.9573637051033309E-2</v>
+        <v>0.1040246946268842</v>
       </c>
       <c r="AD21" s="3">
         <f>'cf1-cor'!AD20/$B21</f>
-        <v>0.55780723759775219</v>
+        <v>0.53310430817123189</v>
       </c>
       <c r="AE21" s="3">
         <f>'cf1-cor'!AE20/$B21</f>
-        <v>2.5282367130554519E-2</v>
+        <v>2.3224886702852943E-2</v>
       </c>
       <c r="AF21" s="3">
         <f>'cf1-cor'!AF20/$B21</f>
-        <v>8.4250452074977625E-2</v>
+        <v>9.0533003333654952E-2</v>
       </c>
       <c r="AG21" s="3">
         <f>'cf1-cor'!AG20/$B21</f>
-        <v>0.10319150555768883</v>
+        <v>0.10924096334176284</v>
       </c>
       <c r="AH21" s="3">
         <f>'cf1-cor'!AH20/$B21</f>
-        <v>0.22599689087442887</v>
+        <v>0.24015330175448832</v>
       </c>
       <c r="AI21" s="3">
         <f>'cf1-cor'!AI20/$B21</f>
-        <v>7.3605756787890983E-2</v>
+        <v>7.562467697504284E-2</v>
       </c>
       <c r="AJ21" s="3">
         <f>'cf1-cor'!AJ20/$B21</f>
-        <v>0.99030132129378867</v>
+        <v>0.98737220179046514</v>
       </c>
       <c r="AK21" s="3">
         <f>'cf1-cor'!AK20/$B21</f>
-        <v>0.15245837442465107</v>
+        <v>0.14846993689466711</v>
       </c>
       <c r="AL21" s="3">
         <f>'cf1-cor'!AL20/$B21</f>
-        <v>0.63025468441022192</v>
+        <v>0.60876862699340528</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
@@ -8667,7 +8692,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>1211335</v>
+        <v>678548</v>
       </c>
       <c r="C22" s="3">
         <f>'cf1-cor'!C21/$B22</f>
@@ -8675,75 +8700,75 @@
       </c>
       <c r="D22" s="3">
         <f>'cf1-cor'!D21/$B22</f>
-        <v>0.40423664799580628</v>
+        <v>0.41922752701356425</v>
       </c>
       <c r="E22" s="3">
         <f>'cf1-cor'!E21/$B22</f>
-        <v>2.3734144559514917E-3</v>
+        <v>1.8038517540395079E-3</v>
       </c>
       <c r="F22" s="3">
         <f>'cf1-cor'!F21/$B22</f>
-        <v>1.9476032641672206E-2</v>
+        <v>2.4522951950341022E-2</v>
       </c>
       <c r="G22" s="3">
         <f>'cf1-cor'!G21/$B22</f>
-        <v>4.9532127776378958E-6</v>
+        <v>8.8424105590171957E-6</v>
       </c>
       <c r="H22" s="3">
         <f>'cf1-cor'!H21/$B22</f>
-        <v>0.64750791482125092</v>
+        <v>0.55998396576218634</v>
       </c>
       <c r="I22" s="3">
         <f>'cf1-cor'!I21/$B22</f>
-        <v>0.13747394403695096</v>
+        <v>0.12260886481133243</v>
       </c>
       <c r="J22" s="3">
         <f>'cf1-cor'!J21/$B22</f>
-        <v>0.13987955437595712</v>
+        <v>0.15253600334832612</v>
       </c>
       <c r="K22" s="3">
         <f>'cf1-cor'!K21/$B22</f>
-        <v>0.38906248065151261</v>
+        <v>0.38366040427501075</v>
       </c>
       <c r="L22" s="3">
         <f>'cf1-cor'!L21/$B22</f>
-        <v>0.16119818217091061</v>
+        <v>0.14591156410452907</v>
       </c>
       <c r="M22" s="3">
         <f>'cf1-cor'!M21/$B22</f>
-        <v>0.3315738420833213</v>
+        <v>0.27914900640780016</v>
       </c>
       <c r="N22" s="3">
         <f>'cf1-cor'!N21/$B22</f>
-        <v>0.9716478100608007</v>
+        <v>0.95749747991299072</v>
       </c>
       <c r="O22" s="3">
         <f>'cf1-cor'!O21/$B22</f>
-        <v>0.50480007594926257</v>
+        <v>0.47451617276891245</v>
       </c>
       <c r="P22" s="3">
         <f>'cf1-cor'!P21/$B22</f>
-        <v>0.50925631637821078</v>
+        <v>0.50985044536274515</v>
       </c>
       <c r="Q22" s="3">
         <f>'cf1-cor'!Q21/$B22</f>
-        <v>0.51893902182302998</v>
+        <v>0.55552444337025531</v>
       </c>
       <c r="R22" s="3">
         <f>'cf1-cor'!R21/$B22</f>
-        <v>0.83978833270730224</v>
+        <v>0.50184953754192774</v>
       </c>
       <c r="S22" s="3">
         <f>'cf1-cor'!S21/$B22</f>
-        <v>0.50131961843750905</v>
+        <v>0.2619239906388347</v>
       </c>
       <c r="T22" s="3">
         <f>'cf1-cor'!T21/$B22</f>
-        <v>0.26004201975506364</v>
+        <v>0.22468565230462695</v>
       </c>
       <c r="U22" s="3">
         <f>'cf1-cor'!U21/$B22</f>
-        <v>1</v>
+        <v>0.17651809451947392</v>
       </c>
       <c r="V22" s="3">
         <f>'cf1-cor'!V21/$B22</f>
@@ -8751,67 +8776,67 @@
       </c>
       <c r="W22" s="3">
         <f>'cf1-cor'!W21/$B22</f>
-        <v>0.45817465853789413</v>
+        <v>3.2740498829854338E-2</v>
       </c>
       <c r="X22" s="3">
         <f>'cf1-cor'!X21/$B22</f>
-        <v>0.51829345309101116</v>
+        <v>0.51403585302734667</v>
       </c>
       <c r="Y22" s="3">
         <f>'cf1-cor'!Y21/$B22</f>
-        <v>0.3962941713068639</v>
+        <v>0.3825167858427112</v>
       </c>
       <c r="Z22" s="3">
         <f>'cf1-cor'!Z21/$B22</f>
-        <v>0.77516459113292357</v>
+        <v>0.76973626036772635</v>
       </c>
       <c r="AA22" s="3">
         <f>'cf1-cor'!AA21/$B22</f>
-        <v>0.99833819711310245</v>
+        <v>0.99768918337391022</v>
       </c>
       <c r="AB22" s="3">
         <f>'cf1-cor'!AB21/$B22</f>
-        <v>0.97894967123050192</v>
+        <v>0.97348897940897328</v>
       </c>
       <c r="AC22" s="3">
         <f>'cf1-cor'!AC21/$B22</f>
-        <v>9.094263766835764E-2</v>
+        <v>9.4056721116265909E-2</v>
       </c>
       <c r="AD22" s="3">
         <f>'cf1-cor'!AD21/$B22</f>
-        <v>0.59258091279456138</v>
+        <v>0.5701969499578512</v>
       </c>
       <c r="AE22" s="3">
         <f>'cf1-cor'!AE21/$B22</f>
-        <v>2.9994179974986275E-2</v>
+        <v>2.6581759875498861E-2</v>
       </c>
       <c r="AF22" s="3">
         <f>'cf1-cor'!AF21/$B22</f>
-        <v>7.3258016981264468E-2</v>
+        <v>8.0518990550410577E-2</v>
       </c>
       <c r="AG22" s="3">
         <f>'cf1-cor'!AG21/$B22</f>
-        <v>9.5716709250537629E-2</v>
+        <v>9.8648879666582173E-2</v>
       </c>
       <c r="AH22" s="3">
         <f>'cf1-cor'!AH21/$B22</f>
-        <v>0.21891466852687325</v>
+        <v>0.2324610786561894</v>
       </c>
       <c r="AI22" s="3">
         <f>'cf1-cor'!AI21/$B22</f>
-        <v>7.5064288574176422E-2</v>
+        <v>7.5667454623696478E-2</v>
       </c>
       <c r="AJ22" s="3">
         <f>'cf1-cor'!AJ21/$B22</f>
-        <v>0.99484535656940487</v>
+        <v>0.99276690816272395</v>
       </c>
       <c r="AK22" s="3">
         <f>'cf1-cor'!AK21/$B22</f>
-        <v>0.16268579707512784</v>
+        <v>0.15252568720267395</v>
       </c>
       <c r="AL22" s="3">
         <f>'cf1-cor'!AL21/$B22</f>
-        <v>0.66184333813519791</v>
+        <v>0.63183739396476002</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.3">
@@ -8883,11 +8908,11 @@
       </c>
       <c r="R23" s="3">
         <f>'cf1-cor'!R22/$B23</f>
-        <v>0.85283142613643526</v>
+        <v>0.41048787123673203</v>
       </c>
       <c r="S23" s="3">
         <f>'cf1-cor'!S22/$B23</f>
-        <v>0.54654479345156692</v>
+        <v>0.24487435203052957</v>
       </c>
       <c r="T23" s="3">
         <f>'cf1-cor'!T22/$B23</f>
@@ -8895,11 +8920,11 @@
       </c>
       <c r="U23" s="3">
         <f>'cf1-cor'!U22/$B23</f>
-        <v>1</v>
+        <v>0.11518135938003939</v>
       </c>
       <c r="V23" s="3">
         <f>'cf1-cor'!V22/$B23</f>
-        <v>1</v>
+        <v>4.0028612457950676E-2</v>
       </c>
       <c r="W23" s="3">
         <f>'cf1-cor'!W22/$B23</f>
@@ -9035,11 +9060,11 @@
       </c>
       <c r="R24" s="3">
         <f>'cf1-cor'!R23/$B24</f>
-        <v>0.76010474669989492</v>
+        <v>0.49030070869514425</v>
       </c>
       <c r="S24" s="3">
         <f>'cf1-cor'!S23/$B24</f>
-        <v>0.36847718157392623</v>
+        <v>0.22476198356761809</v>
       </c>
       <c r="T24" s="3">
         <f>'cf1-cor'!T23/$B24</f>
@@ -9047,11 +9072,11 @@
       </c>
       <c r="U24" s="3">
         <f>'cf1-cor'!U23/$B24</f>
-        <v>0.59172199291304861</v>
+        <v>0.33273577742299754</v>
       </c>
       <c r="V24" s="3">
         <f>'cf1-cor'!V23/$B24</f>
-        <v>0.30558924886102568</v>
+        <v>0.16977434679334916</v>
       </c>
       <c r="W24" s="3">
         <f>'cf1-cor'!W23/$B24</f>
@@ -9187,11 +9212,11 @@
       </c>
       <c r="R25" s="3">
         <f>'cf1-cor'!R24/$B25</f>
-        <v>0.82407207147254069</v>
+        <v>0.49762839602708503</v>
       </c>
       <c r="S25" s="3">
         <f>'cf1-cor'!S24/$B25</f>
-        <v>0.46450080689437168</v>
+        <v>0.25740762307218795</v>
       </c>
       <c r="T25" s="3">
         <f>'cf1-cor'!T24/$B25</f>
@@ -9199,11 +9224,11 @@
       </c>
       <c r="U25" s="3">
         <f>'cf1-cor'!U24/$B25</f>
-        <v>0.68455670720548356</v>
+        <v>0.3555467749180628</v>
       </c>
       <c r="V25" s="3">
         <f>'cf1-cor'!V24/$B25</f>
-        <v>0.39932536975726624</v>
+        <v>0.21591162427005173</v>
       </c>
       <c r="W25" s="3">
         <f>'cf1-cor'!W24/$B25</f>
@@ -9339,11 +9364,11 @@
       </c>
       <c r="R26" s="3">
         <f>'cf1-cor'!R25/$B26</f>
-        <v>0.77226822359229397</v>
+        <v>0.50197777407488109</v>
       </c>
       <c r="S26" s="3">
         <f>'cf1-cor'!S25/$B26</f>
-        <v>0.37766448338182707</v>
+        <v>0.22907571426740325</v>
       </c>
       <c r="T26" s="3">
         <f>'cf1-cor'!T25/$B26</f>
@@ -9351,11 +9376,11 @@
       </c>
       <c r="U26" s="3">
         <f>'cf1-cor'!U25/$B26</f>
-        <v>0.5871306894651166</v>
+        <v>0.33259578040683441</v>
       </c>
       <c r="V26" s="3">
         <f>'cf1-cor'!V25/$B26</f>
-        <v>0.30089083148544549</v>
+        <v>0.16736832997936346</v>
       </c>
       <c r="W26" s="3">
         <f>'cf1-cor'!W25/$B26</f>
@@ -9491,11 +9516,11 @@
       </c>
       <c r="R27" s="3">
         <f>'cf1-cor'!R26/$B27</f>
-        <v>0.76809621750643786</v>
+        <v>0.49222775970458293</v>
       </c>
       <c r="S27" s="3">
         <f>'cf1-cor'!S26/$B27</f>
-        <v>0.37747375827953261</v>
+        <v>0.22715829589209038</v>
       </c>
       <c r="T27" s="3">
         <f>'cf1-cor'!T26/$B27</f>
@@ -9503,11 +9528,11 @@
       </c>
       <c r="U27" s="3">
         <f>'cf1-cor'!U26/$B27</f>
-        <v>0.58082331642523266</v>
+        <v>0.32807521624596803</v>
       </c>
       <c r="V27" s="3">
         <f>'cf1-cor'!V26/$B27</f>
-        <v>0.29795033216681566</v>
+        <v>0.16679297645316207</v>
       </c>
       <c r="W27" s="3">
         <f>'cf1-cor'!W26/$B27</f>
@@ -9643,11 +9668,11 @@
       </c>
       <c r="R28" s="3">
         <f>'cf1-cor'!R27/$B28</f>
-        <v>0.78563959948562367</v>
+        <v>0.50042266460250284</v>
       </c>
       <c r="S28" s="3">
         <f>'cf1-cor'!S27/$B28</f>
-        <v>0.39190008156776573</v>
+        <v>0.23527228443845172</v>
       </c>
       <c r="T28" s="3">
         <f>'cf1-cor'!T27/$B28</f>
@@ -9655,11 +9680,11 @@
       </c>
       <c r="U28" s="3">
         <f>'cf1-cor'!U27/$B28</f>
-        <v>0.59665728221198466</v>
+        <v>0.33560479793250686</v>
       </c>
       <c r="V28" s="3">
         <f>'cf1-cor'!V27/$B28</f>
-        <v>0.30843747789139003</v>
+        <v>0.1718122505628592</v>
       </c>
       <c r="W28" s="3">
         <f>'cf1-cor'!W27/$B28</f>
@@ -9795,11 +9820,11 @@
       </c>
       <c r="R29" s="3">
         <f>'cf1-cor'!R28/$B29</f>
-        <v>0.7072890070765343</v>
+        <v>0.46049597582846691</v>
       </c>
       <c r="S29" s="3">
         <f>'cf1-cor'!S28/$B29</f>
-        <v>0.31189979768709525</v>
+        <v>0.19687740191357969</v>
       </c>
       <c r="T29" s="3">
         <f>'cf1-cor'!T28/$B29</f>
@@ -9807,11 +9832,11 @@
       </c>
       <c r="U29" s="3">
         <f>'cf1-cor'!U28/$B29</f>
-        <v>0.52004355469957864</v>
+        <v>0.30717548214964085</v>
       </c>
       <c r="V29" s="3">
         <f>'cf1-cor'!V28/$B29</f>
-        <v>0.2433099804754795</v>
+        <v>0.14096085377812723</v>
       </c>
       <c r="W29" s="3">
         <f>'cf1-cor'!W28/$B29</f>
@@ -9947,11 +9972,11 @@
       </c>
       <c r="R30" s="3">
         <f>'cf1-cor'!R29/$B30</f>
-        <v>0.81576494979723002</v>
+        <v>0.50237922534323487</v>
       </c>
       <c r="S30" s="3">
         <f>'cf1-cor'!S29/$B30</f>
-        <v>0.43350581545318256</v>
+        <v>0.25036316278420273</v>
       </c>
       <c r="T30" s="3">
         <f>'cf1-cor'!T29/$B30</f>
@@ -9959,11 +9984,11 @@
       </c>
       <c r="U30" s="3">
         <f>'cf1-cor'!U29/$B30</f>
-        <v>0.63954469375049694</v>
+        <v>0.34558405691134175</v>
       </c>
       <c r="V30" s="3">
         <f>'cf1-cor'!V29/$B30</f>
-        <v>0.34804183014648699</v>
+        <v>0.18759660905841441</v>
       </c>
       <c r="W30" s="3">
         <f>'cf1-cor'!W29/$B30</f>
@@ -10099,11 +10124,11 @@
       </c>
       <c r="R31" s="3">
         <f>'cf1-cor'!R30/$B31</f>
-        <v>1</v>
+        <v>0.63206374932468934</v>
       </c>
       <c r="S31" s="3">
         <f>'cf1-cor'!S30/$B31</f>
-        <v>0.59249054565099946</v>
+        <v>0.33184764991896271</v>
       </c>
       <c r="T31" s="3">
         <f>'cf1-cor'!T30/$B31</f>
@@ -10111,11 +10136,11 @@
       </c>
       <c r="U31" s="3">
         <f>'cf1-cor'!U30/$B31</f>
-        <v>0.80745542949756888</v>
+        <v>0.41938141545110752</v>
       </c>
       <c r="V31" s="3">
         <f>'cf1-cor'!V30/$B31</f>
-        <v>0.49072123176661264</v>
+        <v>0.24361156131820638</v>
       </c>
       <c r="W31" s="3">
         <f>'cf1-cor'!W30/$B31</f>
@@ -10251,11 +10276,11 @@
       </c>
       <c r="R32" s="3">
         <f>'cf1-cor'!R31/$B32</f>
-        <v>0.68821434163143891</v>
+        <v>0.47512036167214655</v>
       </c>
       <c r="S32" s="3">
         <f>'cf1-cor'!S31/$B32</f>
-        <v>0.2803913222170033</v>
+        <v>0.18781313605761704</v>
       </c>
       <c r="T32" s="3">
         <f>'cf1-cor'!T31/$B32</f>
@@ -10263,11 +10288,11 @@
       </c>
       <c r="U32" s="3">
         <f>'cf1-cor'!U31/$B32</f>
-        <v>0.48737425630186315</v>
+        <v>0.29610928448410834</v>
       </c>
       <c r="V32" s="3">
         <f>'cf1-cor'!V31/$B32</f>
-        <v>0.21709135744480976</v>
+        <v>0.13366016909347112</v>
       </c>
       <c r="W32" s="3">
         <f>'cf1-cor'!W31/$B32</f>
@@ -10403,11 +10428,11 @@
       </c>
       <c r="R33" s="3">
         <f>'cf1-cor'!R32/$B33</f>
-        <v>0.74209527728249436</v>
+        <v>0.49235358661363327</v>
       </c>
       <c r="S33" s="3">
         <f>'cf1-cor'!S32/$B33</f>
-        <v>0.33071137932610983</v>
+        <v>0.21284003108855667</v>
       </c>
       <c r="T33" s="3">
         <f>'cf1-cor'!T32/$B33</f>
@@ -10415,11 +10440,11 @@
       </c>
       <c r="U33" s="3">
         <f>'cf1-cor'!U32/$B33</f>
-        <v>0.55779271247656925</v>
+        <v>0.33386366753531749</v>
       </c>
       <c r="V33" s="3">
         <f>'cf1-cor'!V32/$B33</f>
-        <v>0.26504137521144788</v>
+        <v>0.15301513281214282</v>
       </c>
       <c r="W33" s="3">
         <f>'cf1-cor'!W32/$B33</f>
@@ -10555,11 +10580,11 @@
       </c>
       <c r="R34" s="3">
         <f>'cf1-cor'!R33/$B34</f>
-        <v>0.63861101766093831</v>
+        <v>0.4481603284563786</v>
       </c>
       <c r="S34" s="3">
         <f>'cf1-cor'!S33/$B34</f>
-        <v>0.23370820202630488</v>
+        <v>0.16750085249443303</v>
       </c>
       <c r="T34" s="3">
         <f>'cf1-cor'!T33/$B34</f>
@@ -10567,11 +10592,11 @@
       </c>
       <c r="U34" s="3">
         <f>'cf1-cor'!U33/$B34</f>
-        <v>0.61151199328074191</v>
+        <v>0.36740564774701168</v>
       </c>
       <c r="V34" s="3">
         <f>'cf1-cor'!V33/$B34</f>
-        <v>0.30344110236112348</v>
+        <v>0.1804953850871833</v>
       </c>
       <c r="W34" s="3">
         <f>'cf1-cor'!W33/$B34</f>
@@ -10707,11 +10732,11 @@
       </c>
       <c r="R35" s="3">
         <f>'cf1-cor'!R34/$B35</f>
-        <v>0.59132731675104555</v>
+        <v>0.41787365177195684</v>
       </c>
       <c r="S35" s="3">
         <f>'cf1-cor'!S34/$B35</f>
-        <v>0.19775478758529605</v>
+        <v>0.14342945190402817</v>
       </c>
       <c r="T35" s="3">
         <f>'cf1-cor'!T34/$B35</f>
@@ -10719,11 +10744,11 @@
       </c>
       <c r="U35" s="3">
         <f>'cf1-cor'!U34/$B35</f>
-        <v>0.63853547582361136</v>
+        <v>0.37092963533641499</v>
       </c>
       <c r="V35" s="3">
         <f>'cf1-cor'!V34/$B35</f>
-        <v>0.33358280137941154</v>
+        <v>0.18836304937999854</v>
       </c>
       <c r="W35" s="3">
         <f>'cf1-cor'!W34/$B35</f>
@@ -10859,11 +10884,11 @@
       </c>
       <c r="R36" s="3">
         <f>'cf1-cor'!R35/$B36</f>
-        <v>0.7763318634393912</v>
+        <v>0.49667090603753999</v>
       </c>
       <c r="S36" s="3">
         <f>'cf1-cor'!S35/$B36</f>
-        <v>0.38324807747709583</v>
+        <v>0.23041365485632145</v>
       </c>
       <c r="T36" s="3">
         <f>'cf1-cor'!T35/$B36</f>
@@ -10871,11 +10896,11 @@
       </c>
       <c r="U36" s="3">
         <f>'cf1-cor'!U35/$B36</f>
-        <v>0.58765258974701295</v>
+        <v>0.33127521413507299</v>
       </c>
       <c r="V36" s="3">
         <f>'cf1-cor'!V35/$B36</f>
-        <v>0.30241679272688582</v>
+        <v>0.16904951431264473</v>
       </c>
       <c r="W36" s="3">
         <f>'cf1-cor'!W35/$B36</f>
@@ -11011,11 +11036,11 @@
       </c>
       <c r="R37" s="3">
         <f>'cf1-cor'!R36/$B37</f>
-        <v>0.73720031654218743</v>
+        <v>0.43871818277631791</v>
       </c>
       <c r="S37" s="3">
         <f>'cf1-cor'!S36/$B37</f>
-        <v>0.3615976448689619</v>
+        <v>0.21652057256265195</v>
       </c>
       <c r="T37" s="3">
         <f>'cf1-cor'!T36/$B37</f>
@@ -11023,11 +11048,11 @@
       </c>
       <c r="U37" s="3">
         <f>'cf1-cor'!U36/$B37</f>
-        <v>0.64400079314182412</v>
+        <v>0.35459155875591059</v>
       </c>
       <c r="V37" s="3">
         <f>'cf1-cor'!V36/$B37</f>
-        <v>0.35203171138212108</v>
+        <v>0.18488064465995829</v>
       </c>
       <c r="W37" s="3">
         <f>'cf1-cor'!W36/$B37</f>
@@ -11163,11 +11188,11 @@
       </c>
       <c r="R38" s="3">
         <f>'cf1-cor'!R37/$B38</f>
-        <v>0.81773955835856182</v>
+        <v>0.51541420155611639</v>
       </c>
       <c r="S38" s="3">
         <f>'cf1-cor'!S37/$B38</f>
-        <v>0.42410594691736964</v>
+        <v>0.24867587347841968</v>
       </c>
       <c r="T38" s="3">
         <f>'cf1-cor'!T37/$B38</f>
@@ -11175,11 +11200,11 @@
       </c>
       <c r="U38" s="3">
         <f>'cf1-cor'!U37/$B38</f>
-        <v>0.6257775333078599</v>
+        <v>0.34175186956503484</v>
       </c>
       <c r="V38" s="3">
         <f>'cf1-cor'!V37/$B38</f>
-        <v>0.33663255751458071</v>
+        <v>0.18002074261936454</v>
       </c>
       <c r="W38" s="3">
         <f>'cf1-cor'!W37/$B38</f>
@@ -11291,4 +11316,92 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CF1: Check that at least one rule is accepted in configuration file
</commit_message>
<xml_diff>
--- a/MGen/cf1-cor.xlsx
+++ b/MGen/cf1-cor.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cf1-cor" sheetId="1" r:id="rId1"/>
     <sheet name="Map" sheetId="2" r:id="rId2"/>
     <sheet name="Flags" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Strict</t>
   </si>
@@ -163,6 +164,36 @@
   </si>
   <si>
     <t>Leap pre/late fill</t>
+  </si>
+  <si>
+    <t>Prepared 3rd</t>
+  </si>
+  <si>
+    <t>Direction change 2</t>
+  </si>
+  <si>
+    <t>Direction change 1</t>
+  </si>
+  <si>
+    <t>Leap2leap</t>
+  </si>
+  <si>
+    <t>Both 3rds</t>
+  </si>
+  <si>
+    <t>Prepared 2 3rds</t>
+  </si>
+  <si>
+    <t>Leap &lt;6</t>
+  </si>
+  <si>
+    <t>Unresolved prepared 3rd</t>
+  </si>
+  <si>
+    <t>Late leap resolve &lt;6</t>
+  </si>
+  <si>
+    <t>Late leap resolve &gt;5</t>
   </si>
 </sst>
 </file>
@@ -5643,7 +5674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
@@ -11548,10 +11579,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E5"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11560,9 +11591,10 @@
     <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>43</v>
       </c>
@@ -11573,7 +11605,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
@@ -11587,7 +11619,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -11601,7 +11633,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
@@ -11615,7 +11647,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0</v>
       </c>
@@ -11627,9 +11659,133 @@
       </c>
       <c r="E5" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CF1: Optimize scan window: check tritone culmination only for full cantus, check fill only if fill search is not cut with scan window, mark leap unresolved only if it is real end of cantus.
</commit_message>
<xml_diff>
--- a/MGen/cf1-cor.xlsx
+++ b/MGen/cf1-cor.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cf1-cor" sheetId="1" r:id="rId1"/>
     <sheet name="Map" sheetId="2" r:id="rId2"/>
-    <sheet name="Flags" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>Strict</t>
   </si>
@@ -139,61 +138,7 @@
     <t>Prepared unfilled 3rd</t>
   </si>
   <si>
-    <t>No flag</t>
-  </si>
-  <si>
-    <t>Pre/late</t>
-  </si>
-  <si>
-    <t>Unfilled</t>
-  </si>
-  <si>
-    <t>Local unfilled</t>
-  </si>
-  <si>
-    <t>Global unfilled</t>
-  </si>
-  <si>
-    <t>3rd prepared</t>
-  </si>
-  <si>
-    <t>No matter</t>
-  </si>
-  <si>
-    <t>3rd prepared unfilled</t>
-  </si>
-  <si>
     <t>Leap pre/late fill</t>
-  </si>
-  <si>
-    <t>Prepared 3rd</t>
-  </si>
-  <si>
-    <t>Direction change 2</t>
-  </si>
-  <si>
-    <t>Direction change 1</t>
-  </si>
-  <si>
-    <t>Leap2leap</t>
-  </si>
-  <si>
-    <t>Both 3rds</t>
-  </si>
-  <si>
-    <t>Prepared 2 3rds</t>
-  </si>
-  <si>
-    <t>Leap &lt;6</t>
-  </si>
-  <si>
-    <t>Unresolved prepared 3rd</t>
-  </si>
-  <si>
-    <t>Late leap resolve &lt;6</t>
-  </si>
-  <si>
-    <t>Late leap resolve &gt;5</t>
   </si>
 </sst>
 </file>
@@ -2216,7 +2161,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3">
         <v>2709779</v>
@@ -5674,8 +5619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL41"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11575,217 +11520,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
CF1: Added blocking flags calculation. Separated calculations into three parameters. Flag statistics sorting by severity. Show full message text in rich edit control on double click. Divide messages into lines. Mutually exclude Leap to leap resolution and 2 thirds after 6/8. Check MAX_WIND
</commit_message>
<xml_diff>
--- a/MGen/cf1-cor.xlsx
+++ b/MGen/cf1-cor.xlsx
@@ -5743,17 +5743,21 @@
   <dimension ref="A1:AM42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA22" sqref="AA22"/>
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" customWidth="1"/>
     <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="16" width="6" customWidth="1"/>
+    <col min="3" max="3" width="2.21875" customWidth="1"/>
+    <col min="4" max="16" width="6" customWidth="1"/>
     <col min="17" max="17" width="7.109375" customWidth="1"/>
-    <col min="18" max="37" width="6" customWidth="1"/>
+    <col min="18" max="20" width="6" customWidth="1"/>
+    <col min="21" max="21" width="3.88671875" customWidth="1"/>
+    <col min="22" max="37" width="6" customWidth="1"/>
     <col min="38" max="38" width="6.21875" customWidth="1"/>
+    <col min="39" max="39" width="6.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">

</xml_diff>